<commit_message>
update A5, add A8
</commit_message>
<xml_diff>
--- a/yuanzd123/evidence.xlsx
+++ b/yuanzd123/evidence.xlsx
@@ -12,12 +12,13 @@
     <sheet name="A4" sheetId="5" r:id="rId8"/>
     <sheet name="A5" sheetId="6" r:id="rId9"/>
     <sheet name="A6" sheetId="7" r:id="rId10"/>
+    <sheet name="A8" sheetId="8" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>TeamName</t>
   </si>
@@ -55,7 +56,7 @@
     <t>juno1d5cz9wyjlkeymw22meq4c9fl7p5k5kyssuyuyg</t>
   </si>
   <si>
-    <t>uptick1vay3r32a9xwzkd2yr03t75p6lyn2wssyq9km0y</t>
+    <t>uptick1vwqum4xggtu4n72n6kvkyxafvqlhv84uzj5hal</t>
   </si>
   <si>
     <t>omniflix1d5cz9wyjlkeymw22meq4c9fl7p5k5kysmsk752</t>
@@ -115,13 +116,19 @@
     <t>gon-flixnet-1</t>
   </si>
   <si>
-    <t>804D9212465BB5CB0E577DDDEA632ACF1C0CFC530961E3AFCC854EFE9A0F09DF</t>
+    <t>61529467796754A7CB19BFF8261770E37F20618272113C18D0B4A7A52A41B7DF</t>
   </si>
   <si>
     <t>Elgafar-1</t>
   </si>
   <si>
     <t>2209CC8073558750DF883BCA3CEBF60783D952B52375C78D562B24B38AAA8A05</t>
+  </si>
+  <si>
+    <t>ibc/1F5C8CFFB36C878178B4B8E08396B4AF03411CE9C38D04E53B754D5847C19561</t>
+  </si>
+  <si>
+    <t>a8a2</t>
   </si>
 </sst>
 </file>
@@ -131,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -149,11 +156,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
@@ -313,7 +315,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -362,7 +364,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -371,20 +373,29 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2019,63 +2030,63 @@
       <c r="D2" t="s" s="20">
         <v>31</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2094,11 +2105,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="17.8516" style="22" customWidth="1"/>
-    <col min="3" max="3" width="16" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="22" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="22" customWidth="1"/>
+    <col min="1" max="1" width="17.8516" style="21" customWidth="1"/>
+    <col min="2" max="2" width="18.0859" style="21" customWidth="1"/>
+    <col min="3" max="3" width="16" style="21" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="21" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
@@ -2204,12 +2216,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.8516" style="23" customWidth="1"/>
-    <col min="2" max="2" width="16" style="23" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="23" customWidth="1"/>
-    <col min="4" max="4" width="14.3516" style="23" customWidth="1"/>
-    <col min="5" max="5" width="12.6719" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="23" customWidth="1"/>
+    <col min="1" max="1" width="17.8516" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16" style="22" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="22" customWidth="1"/>
+    <col min="4" max="4" width="14.3516" style="22" customWidth="1"/>
+    <col min="5" max="5" width="12.6719" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14" customHeight="1">
@@ -2240,63 +2252,63 @@
       <c r="D2" t="s" s="20">
         <v>31</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2305,4 +2317,105 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16" style="23" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="23" customWidth="1"/>
+    <col min="3" max="5" width="8.85156" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17.25" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" ht="17.25" customHeight="1">
+      <c r="A2" t="s" s="26">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s" s="26">
+        <v>36</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>